<commit_message>
modification context dans les extensions b65bd0ad3095a651d87ee70bc2c17d6b7266e32b
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-cp-treatment.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-cp-treatment.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-04T08:55:54+00:00</t>
+    <t>2024-06-10T07:36:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -121,7 +121,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:OncoFAIRCarePlan</t>
+    <t>element:CarePlan</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>